<commit_message>
fix: Fix a few bugs detected during tests
</commit_message>
<xml_diff>
--- a/Freigabe.xlsx
+++ b/Freigabe.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\IdeaProjects\rccitiesv2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B24D46D-9052-49B8-AEFC-CEC8E312B9A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6D26CA-8F77-4A87-9CF8-D99B713A5C91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{187EFE43-8DEF-42E4-9C03-22F226709E54}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{187EFE43-8DEF-42E4-9C03-22F226709E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
   <si>
     <t>RCCities Freigabe</t>
   </si>
@@ -51,13 +52,151 @@
   </si>
   <si>
     <t>Ergebnis</t>
+  </si>
+  <si>
+    <t>Vorhandene Region verhindert das Erstellen</t>
+  </si>
+  <si>
+    <t>Region in Ignorierliste wird ignoriert</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
+  </si>
+  <si>
+    <t>Skipped</t>
+  </si>
+  <si>
+    <t>/town list</t>
+  </si>
+  <si>
+    <t>Zeigt alle Städte an</t>
+  </si>
+  <si>
+    <t>/town invite</t>
+  </si>
+  <si>
+    <t>Man kann sich nicht selbst einladen</t>
+  </si>
+  <si>
+    <t>Town Flag Invite = False verhindert Einladungen</t>
+  </si>
+  <si>
+    <t>Chat Nachricht</t>
+  </si>
+  <si>
+    <t>Chat Nachricht an eingeladenen</t>
+  </si>
+  <si>
+    <t>/town accept</t>
+  </si>
+  <si>
+    <t>Nicht möglich ohne Geld</t>
+  </si>
+  <si>
+    <t>Geld wird abgezogen</t>
+  </si>
+  <si>
+    <t>Spieler ist danach Einwohner in Stadt</t>
+  </si>
+  <si>
+    <t>Bei korrekter Eingabe wir Flagwert gesetzt</t>
+  </si>
+  <si>
+    <t>Bei falscher Einfabe wird Liste an Flags gezeigt</t>
+  </si>
+  <si>
+    <t>/town kick</t>
+  </si>
+  <si>
+    <t>/town flag</t>
+  </si>
+  <si>
+    <t>Einwohner wird aus Stadt geworfen</t>
+  </si>
+  <si>
+    <t>Fehler wenn Spieler kein Einwohner ist</t>
+  </si>
+  <si>
+    <t>Einwohner ohne Leave permission dürfen nicht gekickt werden</t>
+  </si>
+  <si>
+    <t>/town delete</t>
+  </si>
+  <si>
+    <t>Stadt wird gelöscht</t>
+  </si>
+  <si>
+    <t>Ohne -r wird nichts wiederhergestellt</t>
+  </si>
+  <si>
+    <t>Mit -r werden die Chunks wiederhegestellt</t>
+  </si>
+  <si>
+    <t>/town leave</t>
+  </si>
+  <si>
+    <t>Man kann Einwohner nicht nochmals einladen</t>
+  </si>
+  <si>
+    <t>Man verlässt die Stadt</t>
+  </si>
+  <si>
+    <t>/town spawn</t>
+  </si>
+  <si>
+    <t>Man wird erst nach 5s teleportiert</t>
+  </si>
+  <si>
+    <t>Man kann nur jede Minute teleportieren</t>
+  </si>
+  <si>
+    <t>/town setspawn</t>
+  </si>
+  <si>
+    <t>Spawn wird neu gesetzt</t>
+  </si>
+  <si>
+    <t>Spawn muss sich innerhalb der Stadt befinden</t>
+  </si>
+  <si>
+    <t>/town setdesc</t>
+  </si>
+  <si>
+    <t>Beschreibung wird übernommen</t>
+  </si>
+  <si>
+    <t>/town deposit</t>
+  </si>
+  <si>
+    <t>Betrag wird dem Spieler abgezogen</t>
+  </si>
+  <si>
+    <t>Betrag wird der Stadt gutgeschrieben</t>
+  </si>
+  <si>
+    <t>Bei zu wenig Geld kann nichts eingezahlt werden</t>
+  </si>
+  <si>
+    <t>Der Betrag darf nicht negativ sein</t>
+  </si>
+  <si>
+    <t>/town withdraw</t>
+  </si>
+  <si>
+    <t>Der Betrag wir der Stadt abgezogen</t>
+  </si>
+  <si>
+    <t>Der Betrag wird dem Spieler gutgeschrieben</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,13 +224,37 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -106,14 +269,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -428,15 +595,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9BA788-634C-4B4A-87F4-3DAE88B6DAC4}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="70" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
@@ -446,7 +613,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -459,29 +626,390 @@
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B5" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="B11" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>5</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B58" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ABADC70F-E9D6-48B1-A0C5-AB92167E1E57}">
+          <x14:formula1>
+            <xm:f>Tabelle2!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B5:B43</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14D3AB3B-E773-42C6-BBD7-FD8BF71CC94D}">
+  <dimension ref="B2:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: Check if resident is already member of another town. Introduce -u flag for /plot claim command to avoid marking new plot with torches.
</commit_message>
<xml_diff>
--- a/Freigabe.xlsx
+++ b/Freigabe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\IdeaProjects\rccitiesv2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50901C8C-10DB-43C4-B623-A258957108CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0736AB7E-6043-4716-8761-7B2FD038106D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{187EFE43-8DEF-42E4-9C03-22F226709E54}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="100">
   <si>
     <t>RCCities Freigabe</t>
   </si>
@@ -281,6 +281,51 @@
   </si>
   <si>
     <t>Spieler muss Mitglied der Stadt sein</t>
+  </si>
+  <si>
+    <t>Mit der Flag -u wird der Plot nicht markiert</t>
+  </si>
+  <si>
+    <t>Untested</t>
+  </si>
+  <si>
+    <t>Jeder Spieler kann nur in einer Stadt Mitglied sein</t>
+  </si>
+  <si>
+    <t>/resident</t>
+  </si>
+  <si>
+    <t>Mit Spieler als Parameter wird dieser angezeigt</t>
+  </si>
+  <si>
+    <t>Eigene Einwohner Info wird angezeigt</t>
+  </si>
+  <si>
+    <t>/resident setmayor</t>
+  </si>
+  <si>
+    <t>Der Spieler wird Bürgermeister</t>
+  </si>
+  <si>
+    <t>Der Spieler muss Einwohner sein</t>
+  </si>
+  <si>
+    <t>/resident setvicemayor</t>
+  </si>
+  <si>
+    <t>Der Spieler wird Vize-Bürgermeister</t>
+  </si>
+  <si>
+    <t>Der Spieler wird Assistent</t>
+  </si>
+  <si>
+    <t>/resident setassistant</t>
+  </si>
+  <si>
+    <t>/resident setresident</t>
+  </si>
+  <si>
+    <t>Der Spieler wird normaler Einwohner</t>
   </si>
 </sst>
 </file>
@@ -343,7 +388,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -360,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -370,8 +415,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -686,785 +733,726 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9BA788-634C-4B4A-87F4-3DAE88B6DAC4}">
-  <dimension ref="A1:C104"/>
+  <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="75.5703125" style="2" customWidth="1"/>
     <col min="2" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+    </row>
+    <row r="26" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="B27" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="B28" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="B29" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="B32" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+      <c r="B33" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="B36" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="2">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="B37" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="B38" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="B41" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="B42" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
+      <c r="B43" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
+      <c r="B46" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" s="2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="B49" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
+      <c r="B50" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B51" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="2">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="B53" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B52" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="2">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
+      <c r="B54" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" s="2">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
+      <c r="B57" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B58" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C58" s="2">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+      <c r="B60" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B59" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C59" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+      <c r="B61" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B60" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C60" s="2">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+      <c r="B62" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B61" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C61" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
+      <c r="B63" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B64" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C64" s="2">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+      <c r="B66" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B65" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C65" s="2">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+      <c r="B67" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B66" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C66" s="2">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
+      <c r="B68" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B69" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C69" s="2">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+      <c r="B71" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B70" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C70" s="2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
+      <c r="B72" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B73" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C73" s="2">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+      <c r="B75" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B74" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C74" s="2">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="B76" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B75" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C75" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+      <c r="B77" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B76" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C76" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A78" s="3" t="s">
+      <c r="B78" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B79" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
+      <c r="B82" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B80" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C80" s="2">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+      <c r="B83" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B81" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C81" s="2">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+      <c r="B84" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B82" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C82" s="2">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A84" s="3" t="s">
+      <c r="B85" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B85" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C85" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+      <c r="B88" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B86" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C86" s="2">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
+      <c r="B89" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B87" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C87" s="2">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
+      <c r="B90" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B88" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C88" s="2">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A90" s="3" t="s">
+      <c r="B91" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A93" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B91" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C91" s="2">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
+      <c r="B94" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B92" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C92" s="2">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
+      <c r="B95" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B93" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C93" s="2">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A95" s="3" t="s">
+      <c r="B96" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A98" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B96" s="6" t="s">
+      <c r="B99" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C96" s="2">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A98" s="3" t="s">
+    </row>
+    <row r="101" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A101" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B99" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C99" s="2">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
+      <c r="B102" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B100" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C100" s="2">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A102" s="3" t="s">
+      <c r="B103" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A105" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B103" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C103" s="2">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
+      <c r="B106" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B104" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C104" s="2">
-        <v>56</v>
+      <c r="B107" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A109" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A113" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A117" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A121" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A125" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B126" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B127" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ABADC70F-E9D6-48B1-A0C5-AB92167E1E57}">
-          <x14:formula1>
-            <xm:f>Tabelle2!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B5:B43</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fix: NPE with citiy names containing german umlauts
</commit_message>
<xml_diff>
--- a/Freigabe.xlsx
+++ b/Freigabe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\IdeaProjects\rccitiesv2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0736AB7E-6043-4716-8761-7B2FD038106D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A43239-5E6E-4CBC-B2D6-63DD67299222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{187EFE43-8DEF-42E4-9C03-22F226709E54}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="100">
   <si>
     <t>RCCities Freigabe</t>
   </si>
@@ -735,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9BA788-634C-4B4A-87F4-3DAE88B6DAC4}">
   <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A129" sqref="A129"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,6 +821,9 @@
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix: Improve order of intelligent city detection
</commit_message>
<xml_diff>
--- a/Freigabe.xlsx
+++ b/Freigabe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\IdeaProjects\rccitiesv2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A43239-5E6E-4CBC-B2D6-63DD67299222}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1242FC8F-8003-4AC3-95A7-300E0F17A637}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{187EFE43-8DEF-42E4-9C03-22F226709E54}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="99">
   <si>
     <t>RCCities Freigabe</t>
   </si>
@@ -284,9 +284,6 @@
   </si>
   <si>
     <t>Mit der Flag -u wird der Plot nicht markiert</t>
-  </si>
-  <si>
-    <t>Untested</t>
   </si>
   <si>
     <t>Jeder Spieler kann nur in einer Stadt Mitglied sein</t>
@@ -373,7 +370,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -383,12 +380,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -405,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -416,8 +407,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -735,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9BA788-634C-4B4A-87F4-3DAE88B6DAC4}">
   <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,14 +862,14 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" s="9" t="s">
         <v>86</v>
       </c>
+      <c r="B23" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="10"/>
+      <c r="B24" s="8"/>
     </row>
     <row r="26" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
@@ -1186,8 +1175,8 @@
       <c r="A79" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B79" s="8" t="s">
-        <v>86</v>
+      <c r="B79" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
@@ -1350,107 +1339,107 @@
     </row>
     <row r="109" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B110" s="9" t="s">
-        <v>86</v>
+        <v>89</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B111" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B114" s="9" t="s">
-        <v>86</v>
+        <v>91</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B115" s="9" t="s">
-        <v>86</v>
+        <v>92</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="117" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B118" s="9" t="s">
-        <v>86</v>
+        <v>94</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B119" s="9" t="s">
-        <v>86</v>
+        <v>92</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="121" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B122" s="9" t="s">
-        <v>86</v>
+        <v>95</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B123" s="9" t="s">
-        <v>86</v>
+        <v>92</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="125" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B126" s="9" t="s">
-        <v>86</v>
+        <v>98</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B127" s="9" t="s">
-        <v>86</v>
+        <v>92</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: Silent debug comment, increased migration delay to 500ms to decrease pressure
</commit_message>
<xml_diff>
--- a/Freigabe.xlsx
+++ b/Freigabe.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\IdeaProjects\rccitiesv2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1242FC8F-8003-4AC3-95A7-300E0F17A637}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FF3C37-4EF2-4508-A924-38D765B2F8BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{187EFE43-8DEF-42E4-9C03-22F226709E54}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{187EFE43-8DEF-42E4-9C03-22F226709E54}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Befehle" sheetId="1" r:id="rId1"/>
+    <sheet name="Allgemein" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="99">
   <si>
     <t>RCCities Freigabe</t>
   </si>
@@ -55,12 +55,6 @@
     <t>Passed</t>
   </si>
   <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>Skipped</t>
-  </si>
-  <si>
     <t>/town list</t>
   </si>
   <si>
@@ -323,6 +317,13 @@
   </si>
   <si>
     <t>Der Spieler wird normaler Einwohner</t>
+  </si>
+  <si>
+    <t>Queued Confirm Commands wefen keine Exception 
+wenn der Spieler zwischenzeitlich offline gegangen ist</t>
+  </si>
+  <si>
+    <t>Alte Plots werden automatisch migriert</t>
   </si>
 </sst>
 </file>
@@ -396,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -408,6 +409,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -724,7 +729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9BA788-634C-4B4A-87F4-3DAE88B6DAC4}">
   <dimension ref="A1:B127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
@@ -788,7 +793,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>8</v>
@@ -796,7 +801,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>8</v>
@@ -804,12 +809,12 @@
     </row>
     <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>8</v>
@@ -817,12 +822,12 @@
     </row>
     <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>8</v>
@@ -830,7 +835,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>8</v>
@@ -838,7 +843,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>8</v>
@@ -846,7 +851,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>8</v>
@@ -854,7 +859,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>8</v>
@@ -862,7 +867,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>8</v>
@@ -873,12 +878,12 @@
     </row>
     <row r="26" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>8</v>
@@ -886,7 +891,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>8</v>
@@ -894,7 +899,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>8</v>
@@ -902,12 +907,12 @@
     </row>
     <row r="31" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>8</v>
@@ -915,7 +920,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>8</v>
@@ -923,12 +928,12 @@
     </row>
     <row r="35" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>8</v>
@@ -936,7 +941,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>8</v>
@@ -944,7 +949,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>8</v>
@@ -952,12 +957,12 @@
     </row>
     <row r="40" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>8</v>
@@ -965,7 +970,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>8</v>
@@ -973,7 +978,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>8</v>
@@ -981,12 +986,12 @@
     </row>
     <row r="45" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>8</v>
@@ -994,12 +999,12 @@
     </row>
     <row r="48" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>8</v>
@@ -1007,7 +1012,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>8</v>
@@ -1015,12 +1020,12 @@
     </row>
     <row r="52" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>8</v>
@@ -1028,7 +1033,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>8</v>
@@ -1036,12 +1041,12 @@
     </row>
     <row r="56" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>8</v>
@@ -1049,12 +1054,12 @@
     </row>
     <row r="59" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>8</v>
@@ -1062,7 +1067,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>8</v>
@@ -1070,7 +1075,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>8</v>
@@ -1078,7 +1083,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>8</v>
@@ -1086,12 +1091,12 @@
     </row>
     <row r="65" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>8</v>
@@ -1099,7 +1104,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>8</v>
@@ -1107,7 +1112,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>8</v>
@@ -1115,12 +1120,12 @@
     </row>
     <row r="70" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>8</v>
@@ -1128,7 +1133,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>8</v>
@@ -1136,12 +1141,12 @@
     </row>
     <row r="74" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>8</v>
@@ -1149,7 +1154,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>8</v>
@@ -1157,7 +1162,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>8</v>
@@ -1165,7 +1170,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>8</v>
@@ -1173,7 +1178,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>8</v>
@@ -1181,12 +1186,12 @@
     </row>
     <row r="81" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>8</v>
@@ -1194,7 +1199,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>8</v>
@@ -1202,7 +1207,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>8</v>
@@ -1210,7 +1215,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>8</v>
@@ -1218,12 +1223,12 @@
     </row>
     <row r="87" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>8</v>
@@ -1231,7 +1236,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>8</v>
@@ -1239,7 +1244,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>8</v>
@@ -1247,7 +1252,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>8</v>
@@ -1255,12 +1260,12 @@
     </row>
     <row r="93" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>8</v>
@@ -1268,7 +1273,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B95" s="6" t="s">
         <v>8</v>
@@ -1276,7 +1281,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>8</v>
@@ -1284,25 +1289,25 @@
     </row>
     <row r="98" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B102" s="6" t="s">
         <v>8</v>
@@ -1310,7 +1315,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B103" s="6" t="s">
         <v>8</v>
@@ -1318,12 +1323,12 @@
     </row>
     <row r="105" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>8</v>
@@ -1331,7 +1336,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>8</v>
@@ -1339,12 +1344,12 @@
     </row>
     <row r="109" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>8</v>
@@ -1352,7 +1357,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>8</v>
@@ -1360,12 +1365,12 @@
     </row>
     <row r="113" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B114" s="6" t="s">
         <v>8</v>
@@ -1373,7 +1378,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B115" s="6" t="s">
         <v>8</v>
@@ -1381,12 +1386,12 @@
     </row>
     <row r="117" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B118" s="6" t="s">
         <v>8</v>
@@ -1394,7 +1399,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B119" s="6" t="s">
         <v>8</v>
@@ -1402,12 +1407,12 @@
     </row>
     <row r="121" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>8</v>
@@ -1415,7 +1420,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>8</v>
@@ -1423,12 +1428,12 @@
     </row>
     <row r="125" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>8</v>
@@ -1436,7 +1441,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>8</v>
@@ -1450,27 +1455,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14D3AB3B-E773-42C6-BBD7-FD8BF71CC94D}">
-  <dimension ref="B2:B4"/>
+  <dimension ref="A3:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="60.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>10</v>
+    <row r="3" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>